<commit_message>
Config files upto JSON Feedback
</commit_message>
<xml_diff>
--- a/Config Files/AOC-4_NBFC_nodes_seperated_config_new.xlsx
+++ b/Config Files/AOC-4_NBFC_nodes_seperated_config_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC191005-D46C-46DE-A4AB-99B0E72D8FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5982380B-E71B-4916-B9F4-7DAB303EB20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$237</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -2919,8 +2922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="E232" sqref="E232"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E228" sqref="E228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9678,6 +9681,7 @@
       <c r="I253" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I237" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Updated with env variables
</commit_message>
<xml_diff>
--- a/Config Files/AOC-4_NBFC_nodes_seperated_config_new.xlsx
+++ b/Config Files/AOC-4_NBFC_nodes_seperated_config_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC191005-D46C-46DE-A4AB-99B0E72D8FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5982380B-E71B-4916-B9F4-7DAB303EB20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$237</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -2919,8 +2922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="E232" sqref="E232"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E228" sqref="E228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9678,6 +9681,7 @@
       <c r="I253" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I237" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
AOC Config Files updated
</commit_message>
<xml_diff>
--- a/Config Files/AOC-4_NBFC_nodes_seperated_config_new.xlsx
+++ b/Config Files/AOC-4_NBFC_nodes_seperated_config_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCA Portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5982380B-E71B-4916-B9F4-7DAB303EB20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AAFC30-F3C3-446F-8683-C83A47C33FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1993" uniqueCount="367">
   <si>
     <t>Field_Name</t>
   </si>
@@ -1120,13 +1120,19 @@
   </si>
   <si>
     <t>NBFC_IND AS</t>
+  </si>
+  <si>
+    <t>disclosures_auditor_report</t>
+  </si>
+  <si>
+    <t>disclosures_director_report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1152,6 +1158,20 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF343434"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1638,7 +1658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1790,6 +1810,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2922,11 +2944,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I253"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E228" sqref="E228"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="44" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="1" customWidth="1"/>
@@ -2941,7 +2963,7 @@
     <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2970,7 +2992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2983,7 +3005,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.7" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -3010,7 +3032,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.7" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
@@ -3037,7 +3059,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.5" customHeight="1">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -3064,7 +3086,7 @@
       </c>
       <c r="I5" s="21"/>
     </row>
-    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.5" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
@@ -3091,7 +3113,7 @@
       </c>
       <c r="I6" s="21"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.5" customHeight="1">
       <c r="A7" s="26" t="s">
         <v>23</v>
       </c>
@@ -3104,7 +3126,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.7" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
@@ -3131,7 +3153,7 @@
       </c>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.7" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>17</v>
       </c>
@@ -3158,7 +3180,7 @@
       </c>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.5" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>19</v>
       </c>
@@ -3185,7 +3207,7 @@
       </c>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.5" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>22</v>
       </c>
@@ -3212,7 +3234,7 @@
       </c>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.5" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>26</v>
       </c>
@@ -3225,7 +3247,7 @@
       <c r="H12" s="11"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="28" t="s">
         <v>27</v>
       </c>
@@ -3254,7 +3276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="12" t="s">
         <v>30</v>
       </c>
@@ -3283,7 +3305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>32</v>
       </c>
@@ -3312,7 +3334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="12" t="s">
         <v>34</v>
       </c>
@@ -3341,7 +3363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>36</v>
       </c>
@@ -3370,7 +3392,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>38</v>
       </c>
@@ -3399,7 +3421,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.5" customHeight="1">
       <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
@@ -3428,7 +3450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="12" t="s">
         <v>42</v>
       </c>
@@ -3457,7 +3479,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="12" t="s">
         <v>44</v>
       </c>
@@ -3486,7 +3508,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="24" customHeight="1">
       <c r="A22" s="12" t="s">
         <v>46</v>
       </c>
@@ -3515,7 +3537,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="12" t="s">
         <v>48</v>
       </c>
@@ -3544,7 +3566,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="12" t="s">
         <v>50</v>
       </c>
@@ -3573,7 +3595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="12" t="s">
         <v>52</v>
       </c>
@@ -3602,7 +3624,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>54</v>
       </c>
@@ -3631,7 +3653,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="12" t="s">
         <v>56</v>
       </c>
@@ -3660,7 +3682,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="12" t="s">
         <v>58</v>
       </c>
@@ -3689,7 +3711,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="12" t="s">
         <v>60</v>
       </c>
@@ -3718,7 +3740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="12" t="s">
         <v>62</v>
       </c>
@@ -3747,7 +3769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="12" t="s">
         <v>64</v>
       </c>
@@ -3776,7 +3798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="12" t="s">
         <v>66</v>
       </c>
@@ -3805,7 +3827,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13.5" customHeight="1">
       <c r="A33" s="27" t="s">
         <v>68</v>
       </c>
@@ -3818,7 +3840,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="28" t="s">
         <v>27</v>
       </c>
@@ -3847,7 +3869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="12" t="s">
         <v>30</v>
       </c>
@@ -3876,7 +3898,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="12" t="s">
         <v>32</v>
       </c>
@@ -3905,7 +3927,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="12" t="s">
         <v>34</v>
       </c>
@@ -3934,7 +3956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
@@ -3963,7 +3985,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="12" t="s">
         <v>38</v>
       </c>
@@ -3992,7 +4014,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="13.5" customHeight="1">
       <c r="A40" s="12" t="s">
         <v>40</v>
       </c>
@@ -4021,7 +4043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="12" t="s">
         <v>42</v>
       </c>
@@ -4050,7 +4072,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="12" t="s">
         <v>44</v>
       </c>
@@ -4079,7 +4101,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="12" t="s">
         <v>46</v>
       </c>
@@ -4108,7 +4130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="12" t="s">
         <v>48</v>
       </c>
@@ -4137,7 +4159,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -4166,7 +4188,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="12" t="s">
         <v>52</v>
       </c>
@@ -4195,7 +4217,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="12" t="s">
         <v>54</v>
       </c>
@@ -4224,7 +4246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="12" t="s">
         <v>56</v>
       </c>
@@ -4253,7 +4275,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="12" t="s">
         <v>58</v>
       </c>
@@ -4282,7 +4304,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="12" t="s">
         <v>60</v>
       </c>
@@ -4311,7 +4333,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="12" t="s">
         <v>62</v>
       </c>
@@ -4340,7 +4362,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="12" t="s">
         <v>64</v>
       </c>
@@ -4369,7 +4391,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="12" t="s">
         <v>66</v>
       </c>
@@ -4398,7 +4420,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1">
       <c r="A54" s="27" t="s">
         <v>89</v>
       </c>
@@ -4411,7 +4433,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="12" t="s">
         <v>90</v>
       </c>
@@ -4440,7 +4462,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="12" t="s">
         <v>93</v>
       </c>
@@ -4469,7 +4491,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="12" t="s">
         <v>95</v>
       </c>
@@ -4498,7 +4520,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="12" t="s">
         <v>97</v>
       </c>
@@ -4527,7 +4549,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A59" s="12" t="s">
         <v>99</v>
       </c>
@@ -4556,7 +4578,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A60" s="12" t="s">
         <v>101</v>
       </c>
@@ -4585,7 +4607,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A61" s="12" t="s">
         <v>103</v>
       </c>
@@ -4614,7 +4636,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A62" s="12" t="s">
         <v>105</v>
       </c>
@@ -4643,7 +4665,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A63" s="12" t="s">
         <v>107</v>
       </c>
@@ -4672,7 +4694,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A64" s="12" t="s">
         <v>109</v>
       </c>
@@ -4701,7 +4723,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A65" s="12" t="s">
         <v>111</v>
       </c>
@@ -4730,7 +4752,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A66" s="12" t="s">
         <v>113</v>
       </c>
@@ -4759,7 +4781,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A67" s="12" t="s">
         <v>115</v>
       </c>
@@ -4788,7 +4810,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A68" s="12" t="s">
         <v>117</v>
       </c>
@@ -4817,7 +4839,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A69" s="12" t="s">
         <v>119</v>
       </c>
@@ -4846,7 +4868,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A70" s="12" t="s">
         <v>121</v>
       </c>
@@ -4875,7 +4897,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1">
       <c r="A71" s="28" t="s">
         <v>123</v>
       </c>
@@ -4904,7 +4926,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A72" s="35" t="s">
         <v>125</v>
       </c>
@@ -4933,7 +4955,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A73" s="12" t="s">
         <v>128</v>
       </c>
@@ -4962,7 +4984,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A74" s="12" t="s">
         <v>130</v>
       </c>
@@ -4991,7 +5013,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A75" s="12" t="s">
         <v>132</v>
       </c>
@@ -5020,7 +5042,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A76" s="12" t="s">
         <v>134</v>
       </c>
@@ -5049,7 +5071,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A77" s="12" t="s">
         <v>136</v>
       </c>
@@ -5078,7 +5100,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A78" s="12" t="s">
         <v>138</v>
       </c>
@@ -5107,7 +5129,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A79" s="12" t="s">
         <v>140</v>
       </c>
@@ -5136,7 +5158,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A80" s="12" t="s">
         <v>142</v>
       </c>
@@ -5165,7 +5187,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A81" s="12" t="s">
         <v>144</v>
       </c>
@@ -5194,7 +5216,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A82" s="12" t="s">
         <v>146</v>
       </c>
@@ -5223,7 +5245,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30" customHeight="1">
       <c r="A83" s="12" t="s">
         <v>148</v>
       </c>
@@ -5252,7 +5274,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A84" s="12" t="s">
         <v>150</v>
       </c>
@@ -5281,7 +5303,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A85" s="12" t="s">
         <v>152</v>
       </c>
@@ -5310,7 +5332,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="13.5" customHeight="1">
       <c r="A86" s="28" t="s">
         <v>154</v>
       </c>
@@ -5339,7 +5361,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="45.75" customHeight="1">
       <c r="A87" s="37" t="s">
         <v>156</v>
       </c>
@@ -5368,7 +5390,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="237.75" customHeight="1">
       <c r="A88" s="42" t="s">
         <v>159</v>
       </c>
@@ -5397,7 +5419,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="13.5" customHeight="1">
       <c r="A89" s="27" t="s">
         <v>162</v>
       </c>
@@ -5410,7 +5432,7 @@
       <c r="H89" s="10"/>
       <c r="I89" s="11"/>
     </row>
-    <row r="90" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A90" s="12" t="s">
         <v>90</v>
       </c>
@@ -5439,7 +5461,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A91" s="12" t="s">
         <v>93</v>
       </c>
@@ -5468,7 +5490,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A92" s="12" t="s">
         <v>95</v>
       </c>
@@ -5497,7 +5519,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A93" s="12" t="s">
         <v>97</v>
       </c>
@@ -5526,7 +5548,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A94" s="12" t="s">
         <v>99</v>
       </c>
@@ -5555,7 +5577,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A95" s="12" t="s">
         <v>101</v>
       </c>
@@ -5584,7 +5606,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A96" s="12" t="s">
         <v>103</v>
       </c>
@@ -5613,7 +5635,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A97" s="12" t="s">
         <v>105</v>
       </c>
@@ -5642,7 +5664,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A98" s="12" t="s">
         <v>107</v>
       </c>
@@ -5671,7 +5693,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A99" s="12" t="s">
         <v>109</v>
       </c>
@@ -5700,7 +5722,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A100" s="12" t="s">
         <v>111</v>
       </c>
@@ -5729,7 +5751,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A101" s="12" t="s">
         <v>113</v>
       </c>
@@ -5758,7 +5780,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A102" s="12" t="s">
         <v>115</v>
       </c>
@@ -5787,7 +5809,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A103" s="12" t="s">
         <v>117</v>
       </c>
@@ -5816,7 +5838,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A104" s="12" t="s">
         <v>119</v>
       </c>
@@ -5845,7 +5867,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A105" s="12" t="s">
         <v>121</v>
       </c>
@@ -5874,7 +5896,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="13.5" customHeight="1">
       <c r="A106" s="28" t="s">
         <v>123</v>
       </c>
@@ -5903,7 +5925,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A107" s="35" t="s">
         <v>125</v>
       </c>
@@ -5932,7 +5954,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A108" s="12" t="s">
         <v>128</v>
       </c>
@@ -5961,7 +5983,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A109" s="12" t="s">
         <v>130</v>
       </c>
@@ -5990,7 +6012,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A110" s="12" t="s">
         <v>132</v>
       </c>
@@ -6019,7 +6041,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A111" s="12" t="s">
         <v>134</v>
       </c>
@@ -6048,7 +6070,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A112" s="12" t="s">
         <v>136</v>
       </c>
@@ -6077,7 +6099,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A113" s="12" t="s">
         <v>138</v>
       </c>
@@ -6106,7 +6128,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A114" s="12" t="s">
         <v>140</v>
       </c>
@@ -6135,7 +6157,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A115" s="12" t="s">
         <v>142</v>
       </c>
@@ -6164,7 +6186,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A116" s="12" t="s">
         <v>144</v>
       </c>
@@ -6193,7 +6215,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A117" s="12" t="s">
         <v>146</v>
       </c>
@@ -6222,7 +6244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="30" customHeight="1">
       <c r="A118" s="12" t="s">
         <v>148</v>
       </c>
@@ -6251,7 +6273,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A119" s="12" t="s">
         <v>150</v>
       </c>
@@ -6280,7 +6302,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A120" s="12" t="s">
         <v>152</v>
       </c>
@@ -6309,7 +6331,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="13.5" customHeight="1">
       <c r="A121" s="28" t="s">
         <v>154</v>
       </c>
@@ -6338,7 +6360,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="45" customHeight="1">
       <c r="A122" s="37" t="s">
         <v>194</v>
       </c>
@@ -6367,7 +6389,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="178.5" customHeight="1">
       <c r="A123" s="42" t="s">
         <v>159</v>
       </c>
@@ -6396,7 +6418,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="21.75" customHeight="1">
       <c r="A124" s="43" t="s">
         <v>197</v>
       </c>
@@ -6409,7 +6431,7 @@
       <c r="H124" s="45"/>
       <c r="I124" s="46"/>
     </row>
-    <row r="125" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="21.75" customHeight="1">
       <c r="A125" s="17" t="s">
         <v>198</v>
       </c>
@@ -6438,7 +6460,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="84.75" customHeight="1">
       <c r="A126" s="48" t="s">
         <v>201</v>
       </c>
@@ -6467,7 +6489,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="30" customHeight="1">
       <c r="A127" s="17" t="s">
         <v>203</v>
       </c>
@@ -6496,7 +6518,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="46.5" customHeight="1">
       <c r="A128" s="17" t="s">
         <v>205</v>
       </c>
@@ -6525,7 +6547,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="66" customHeight="1">
       <c r="A129" s="17" t="s">
         <v>207</v>
       </c>
@@ -6554,7 +6576,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="33" customHeight="1">
       <c r="A130" s="17" t="s">
         <v>209</v>
       </c>
@@ -6583,7 +6605,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="25.5" customHeight="1">
       <c r="A131" s="17" t="s">
         <v>211</v>
       </c>
@@ -6612,7 +6634,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="25.5" customHeight="1">
       <c r="A132" s="43" t="s">
         <v>213</v>
       </c>
@@ -6625,7 +6647,7 @@
       <c r="H132" s="10"/>
       <c r="I132" s="11"/>
     </row>
-    <row r="133" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="21.75" customHeight="1">
       <c r="A133" s="17" t="s">
         <v>198</v>
       </c>
@@ -6654,7 +6676,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="84.75" customHeight="1">
       <c r="A134" s="48" t="s">
         <v>201</v>
       </c>
@@ -6683,7 +6705,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="30" customHeight="1">
       <c r="A135" s="17" t="s">
         <v>203</v>
       </c>
@@ -6712,7 +6734,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="46.5" customHeight="1">
       <c r="A136" s="17" t="s">
         <v>205</v>
       </c>
@@ -6741,7 +6763,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="66" customHeight="1">
       <c r="A137" s="17" t="s">
         <v>207</v>
       </c>
@@ -6770,7 +6792,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="33" customHeight="1">
       <c r="A138" s="17" t="s">
         <v>209</v>
       </c>
@@ -6799,7 +6821,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="25.5" customHeight="1">
       <c r="A139" s="17" t="s">
         <v>211</v>
       </c>
@@ -6828,7 +6850,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="13.5" customHeight="1">
       <c r="A140" s="55" t="s">
         <v>214</v>
       </c>
@@ -6841,7 +6863,7 @@
       <c r="H140" s="10"/>
       <c r="I140" s="56"/>
     </row>
-    <row r="141" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="13.5" customHeight="1">
       <c r="A141" s="17" t="s">
         <v>215</v>
       </c>
@@ -6870,7 +6892,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="13.5" customHeight="1">
       <c r="A142" s="17" t="s">
         <v>219</v>
       </c>
@@ -6899,7 +6921,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A143" s="12" t="s">
         <v>221</v>
       </c>
@@ -6928,7 +6950,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A144" s="12" t="s">
         <v>223</v>
       </c>
@@ -6957,7 +6979,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A145" s="12" t="s">
         <v>225</v>
       </c>
@@ -6986,7 +7008,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A146" s="12" t="s">
         <v>227</v>
       </c>
@@ -7015,7 +7037,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A147" s="12" t="s">
         <v>229</v>
       </c>
@@ -7044,7 +7066,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A148" s="12" t="s">
         <v>231</v>
       </c>
@@ -7073,7 +7095,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A149" s="12" t="s">
         <v>233</v>
       </c>
@@ -7102,7 +7124,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" ht="13.5" customHeight="1">
       <c r="A150" s="55" t="s">
         <v>235</v>
       </c>
@@ -7115,7 +7137,7 @@
       <c r="H150" s="10"/>
       <c r="I150" s="10"/>
     </row>
-    <row r="151" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" ht="13.5" customHeight="1">
       <c r="A151" s="17" t="s">
         <v>215</v>
       </c>
@@ -7144,7 +7166,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" ht="13.5" customHeight="1">
       <c r="A152" s="17" t="s">
         <v>219</v>
       </c>
@@ -7173,7 +7195,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A153" s="12" t="s">
         <v>221</v>
       </c>
@@ -7202,7 +7224,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A154" s="12" t="s">
         <v>223</v>
       </c>
@@ -7231,7 +7253,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A155" s="12" t="s">
         <v>225</v>
       </c>
@@ -7260,7 +7282,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A156" s="12" t="s">
         <v>227</v>
       </c>
@@ -7289,7 +7311,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A157" s="12" t="s">
         <v>229</v>
       </c>
@@ -7318,7 +7340,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A158" s="12" t="s">
         <v>231</v>
       </c>
@@ -7347,7 +7369,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A159" s="12" t="s">
         <v>233</v>
       </c>
@@ -7376,7 +7398,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" ht="13.5" customHeight="1">
       <c r="A160" s="59" t="s">
         <v>245</v>
       </c>
@@ -7389,7 +7411,7 @@
       <c r="H160" s="10"/>
       <c r="I160" s="60"/>
     </row>
-    <row r="161" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="13.5" customHeight="1">
       <c r="A161" s="61" t="s">
         <v>246</v>
       </c>
@@ -7418,7 +7440,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="45.75" customHeight="1">
       <c r="A162" s="63" t="s">
         <v>249</v>
       </c>
@@ -7447,7 +7469,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="30.75" customHeight="1">
       <c r="A163" s="64" t="s">
         <v>251</v>
       </c>
@@ -7476,7 +7498,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" ht="13.5" customHeight="1">
       <c r="A164" s="63" t="s">
         <v>253</v>
       </c>
@@ -7505,7 +7527,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="13.5" customHeight="1">
       <c r="A165" s="63" t="s">
         <v>256</v>
       </c>
@@ -7534,7 +7556,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" ht="45.75" customHeight="1">
       <c r="A166" s="42" t="s">
         <v>258</v>
       </c>
@@ -7563,7 +7585,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" ht="30.75" customHeight="1">
       <c r="A167" s="12" t="s">
         <v>260</v>
       </c>
@@ -7592,7 +7614,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" ht="30.75" customHeight="1">
       <c r="A168" s="12" t="s">
         <v>262</v>
       </c>
@@ -7621,7 +7643,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" ht="13.5" customHeight="1">
       <c r="A169" s="12" t="s">
         <v>264</v>
       </c>
@@ -7650,7 +7672,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="13.5" customHeight="1">
       <c r="A170" s="28" t="s">
         <v>266</v>
       </c>
@@ -7679,7 +7701,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" ht="13.5" customHeight="1">
       <c r="A171" s="28" t="s">
         <v>269</v>
       </c>
@@ -7708,7 +7730,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" ht="13.5" customHeight="1">
       <c r="A172" s="12" t="s">
         <v>272</v>
       </c>
@@ -7737,7 +7759,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="13.5" customHeight="1">
       <c r="A173" s="12" t="s">
         <v>274</v>
       </c>
@@ -7766,7 +7788,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" ht="13.5" customHeight="1">
       <c r="A174" s="12" t="s">
         <v>276</v>
       </c>
@@ -7795,7 +7817,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" ht="13.5" customHeight="1">
       <c r="A175" s="12" t="s">
         <v>277</v>
       </c>
@@ -7824,7 +7846,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" ht="45.75" customHeight="1">
       <c r="A176" s="17" t="s">
         <v>278</v>
       </c>
@@ -7853,7 +7875,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" ht="26.65" customHeight="1">
       <c r="A177" s="12" t="s">
         <v>280</v>
       </c>
@@ -7882,7 +7904,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" ht="13.5" customHeight="1">
       <c r="A178" s="12" t="s">
         <v>282</v>
       </c>
@@ -7911,7 +7933,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" ht="13.5" customHeight="1">
       <c r="A179" s="12" t="s">
         <v>284</v>
       </c>
@@ -7940,7 +7962,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="30.75" customHeight="1">
       <c r="A180" s="12" t="s">
         <v>286</v>
       </c>
@@ -7969,7 +7991,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" ht="30.75" customHeight="1">
       <c r="A181" s="12" t="s">
         <v>288</v>
       </c>
@@ -7998,7 +8020,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" ht="30.75" customHeight="1">
       <c r="A182" s="12" t="s">
         <v>290</v>
       </c>
@@ -8027,7 +8049,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" ht="30.75" customHeight="1">
       <c r="A183" s="12" t="s">
         <v>292</v>
       </c>
@@ -8056,7 +8078,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" ht="13.5" customHeight="1">
       <c r="A184" s="12" t="s">
         <v>294</v>
       </c>
@@ -8085,7 +8107,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" ht="13.5" customHeight="1">
       <c r="A185" s="12" t="s">
         <v>296</v>
       </c>
@@ -8114,7 +8136,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" ht="30.75" customHeight="1">
       <c r="A186" s="12" t="s">
         <v>298</v>
       </c>
@@ -8143,7 +8165,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" ht="30.75" customHeight="1">
       <c r="A187" s="12" t="s">
         <v>300</v>
       </c>
@@ -8172,7 +8194,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="30.75" customHeight="1">
       <c r="A188" s="12" t="s">
         <v>301</v>
       </c>
@@ -8201,7 +8223,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" ht="13.5" customHeight="1">
       <c r="A189" s="59" t="s">
         <v>303</v>
       </c>
@@ -8214,7 +8236,7 @@
       <c r="H189" s="10"/>
       <c r="I189" s="69"/>
     </row>
-    <row r="190" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" ht="13.5" customHeight="1">
       <c r="A190" s="61" t="s">
         <v>246</v>
       </c>
@@ -8243,7 +8265,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" ht="45.75" customHeight="1">
       <c r="A191" s="63" t="s">
         <v>249</v>
       </c>
@@ -8272,7 +8294,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" ht="30.75" customHeight="1">
       <c r="A192" s="64" t="s">
         <v>251</v>
       </c>
@@ -8301,7 +8323,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" ht="13.5" customHeight="1">
       <c r="A193" s="63" t="s">
         <v>253</v>
       </c>
@@ -8330,7 +8352,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" ht="13.5" customHeight="1">
       <c r="A194" s="63" t="s">
         <v>256</v>
       </c>
@@ -8359,7 +8381,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="45.75" customHeight="1">
       <c r="A195" s="42" t="s">
         <v>258</v>
       </c>
@@ -8388,7 +8410,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" ht="30.75" customHeight="1">
       <c r="A196" s="12" t="s">
         <v>260</v>
       </c>
@@ -8417,7 +8439,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" ht="30.75" customHeight="1">
       <c r="A197" s="12" t="s">
         <v>262</v>
       </c>
@@ -8446,7 +8468,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" ht="13.5" customHeight="1">
       <c r="A198" s="12" t="s">
         <v>264</v>
       </c>
@@ -8475,7 +8497,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" ht="13.5" customHeight="1">
       <c r="A199" s="28" t="s">
         <v>312</v>
       </c>
@@ -8504,7 +8526,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" ht="13.5" customHeight="1">
       <c r="A200" s="28" t="s">
         <v>271</v>
       </c>
@@ -8533,7 +8555,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="13.5" customHeight="1">
       <c r="A201" s="28" t="s">
         <v>272</v>
       </c>
@@ -8562,7 +8584,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" ht="13.5" customHeight="1">
       <c r="A202" s="12" t="s">
         <v>274</v>
       </c>
@@ -8591,7 +8613,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" ht="13.5" customHeight="1">
       <c r="A203" s="12" t="s">
         <v>276</v>
       </c>
@@ -8620,7 +8642,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" ht="13.5" customHeight="1">
       <c r="A204" s="12" t="s">
         <v>277</v>
       </c>
@@ -8649,7 +8671,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" ht="45.75" customHeight="1">
       <c r="A205" s="17" t="s">
         <v>278</v>
       </c>
@@ -8678,7 +8700,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="26.65" customHeight="1">
       <c r="A206" s="12" t="s">
         <v>280</v>
       </c>
@@ -8707,7 +8729,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" ht="13.5" customHeight="1">
       <c r="A207" s="12" t="s">
         <v>282</v>
       </c>
@@ -8736,7 +8758,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" ht="13.5" customHeight="1">
       <c r="A208" s="12" t="s">
         <v>284</v>
       </c>
@@ -8765,7 +8787,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" ht="30.75" customHeight="1">
       <c r="A209" s="12" t="s">
         <v>286</v>
       </c>
@@ -8794,7 +8816,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" ht="30.75" customHeight="1">
       <c r="A210" s="12" t="s">
         <v>288</v>
       </c>
@@ -8823,7 +8845,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" ht="30.75" customHeight="1">
       <c r="A211" s="12" t="s">
         <v>290</v>
       </c>
@@ -8852,7 +8874,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" ht="30.75" customHeight="1">
       <c r="A212" s="12" t="s">
         <v>292</v>
       </c>
@@ -8881,7 +8903,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" ht="13.5" customHeight="1">
       <c r="A213" s="12" t="s">
         <v>294</v>
       </c>
@@ -8910,7 +8932,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" ht="13.5" customHeight="1">
       <c r="A214" s="12" t="s">
         <v>296</v>
       </c>
@@ -8939,7 +8961,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" ht="30.75" customHeight="1">
       <c r="A215" s="12" t="s">
         <v>298</v>
       </c>
@@ -8968,7 +8990,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" ht="30.75" customHeight="1">
       <c r="A216" s="12" t="s">
         <v>300</v>
       </c>
@@ -8997,7 +9019,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" ht="30.75" customHeight="1">
       <c r="A217" s="12" t="s">
         <v>301</v>
       </c>
@@ -9026,7 +9048,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" ht="29.25" customHeight="1">
       <c r="A218" s="71" t="s">
         <v>328</v>
       </c>
@@ -9039,7 +9061,7 @@
       <c r="H218" s="10"/>
       <c r="I218" s="11"/>
     </row>
-    <row r="219" spans="1:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="30.95" customHeight="1">
       <c r="A219" s="17" t="s">
         <v>329</v>
       </c>
@@ -9068,7 +9090,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="29.25" customHeight="1">
       <c r="A220" s="71" t="s">
         <v>328</v>
       </c>
@@ -9081,7 +9103,7 @@
       <c r="H220" s="45"/>
       <c r="I220" s="74"/>
     </row>
-    <row r="221" spans="1:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" ht="30.95" customHeight="1">
       <c r="A221" s="17" t="s">
         <v>329</v>
       </c>
@@ -9110,7 +9132,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" ht="14.45" customHeight="1">
       <c r="A222" s="55" t="s">
         <v>331</v>
       </c>
@@ -9123,7 +9145,7 @@
       <c r="H222" s="10"/>
       <c r="I222" s="10"/>
     </row>
-    <row r="223" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="13.7" customHeight="1">
       <c r="A223" s="12" t="s">
         <v>332</v>
       </c>
@@ -9152,7 +9174,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" ht="24" customHeight="1">
       <c r="A224" s="76" t="s">
         <v>338</v>
       </c>
@@ -9165,7 +9187,7 @@
       <c r="H224" s="10"/>
       <c r="I224" s="10"/>
     </row>
-    <row r="225" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" ht="24.6" customHeight="1">
       <c r="A225" s="12" t="s">
         <v>339</v>
       </c>
@@ -9194,7 +9216,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" ht="13.5" customHeight="1">
       <c r="A226" s="55" t="s">
         <v>342</v>
       </c>
@@ -9207,7 +9229,7 @@
       <c r="H226" s="10"/>
       <c r="I226" s="10"/>
     </row>
-    <row r="227" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A227" s="17" t="s">
         <v>10</v>
       </c>
@@ -9234,7 +9256,7 @@
       </c>
       <c r="I227" s="10"/>
     </row>
-    <row r="228" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A228" s="17" t="s">
         <v>17</v>
       </c>
@@ -9261,7 +9283,7 @@
       </c>
       <c r="I228" s="10"/>
     </row>
-    <row r="229" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A229" s="12" t="s">
         <v>345</v>
       </c>
@@ -9288,7 +9310,7 @@
       </c>
       <c r="I229" s="10"/>
     </row>
-    <row r="230" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A230" s="12" t="s">
         <v>347</v>
       </c>
@@ -9315,7 +9337,7 @@
       </c>
       <c r="I230" s="10"/>
     </row>
-    <row r="231" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A231" s="12" t="s">
         <v>349</v>
       </c>
@@ -9342,7 +9364,7 @@
       </c>
       <c r="I231" s="10"/>
     </row>
-    <row r="232" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A232" s="12" t="s">
         <v>351</v>
       </c>
@@ -9369,7 +9391,7 @@
       </c>
       <c r="I232" s="10"/>
     </row>
-    <row r="233" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A233" s="12" t="s">
         <v>352</v>
       </c>
@@ -9396,7 +9418,7 @@
       </c>
       <c r="I233" s="10"/>
     </row>
-    <row r="234" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A234" s="77" t="s">
         <v>354</v>
       </c>
@@ -9423,7 +9445,7 @@
       </c>
       <c r="I234" s="10"/>
     </row>
-    <row r="235" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" ht="17.100000000000001" customHeight="1">
       <c r="A235" s="77" t="s">
         <v>356</v>
       </c>
@@ -9450,7 +9472,7 @@
       </c>
       <c r="I235" s="10"/>
     </row>
-    <row r="236" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" ht="45.75" customHeight="1">
       <c r="A236" s="12" t="s">
         <v>358</v>
       </c>
@@ -9477,7 +9499,7 @@
       </c>
       <c r="I236" s="21"/>
     </row>
-    <row r="237" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" ht="30.75" customHeight="1">
       <c r="A237" s="77" t="s">
         <v>360</v>
       </c>
@@ -9504,29 +9526,51 @@
       </c>
       <c r="I237" s="21"/>
     </row>
-    <row r="238" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="11"/>
-      <c r="B238" s="10"/>
-      <c r="C238" s="10"/>
-      <c r="D238" s="10"/>
-      <c r="E238" s="10"/>
-      <c r="F238" s="10"/>
-      <c r="G238" s="10"/>
-      <c r="H238" s="11"/>
-      <c r="I238" s="10"/>
-    </row>
-    <row r="239" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="10"/>
-      <c r="B239" s="10"/>
-      <c r="C239" s="10"/>
-      <c r="D239" s="10"/>
-      <c r="E239" s="10"/>
-      <c r="F239" s="10"/>
-      <c r="G239" s="10"/>
-      <c r="H239" s="10"/>
-      <c r="I239" s="10"/>
-    </row>
-    <row r="240" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" ht="13.5" customHeight="1">
+      <c r="A238" t="s">
+        <v>365</v>
+      </c>
+      <c r="B238"/>
+      <c r="C238" t="s">
+        <v>12</v>
+      </c>
+      <c r="D238" t="s">
+        <v>20</v>
+      </c>
+      <c r="E238"/>
+      <c r="F238" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="G238" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="H238" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="13.5" customHeight="1">
+      <c r="A239" t="s">
+        <v>366</v>
+      </c>
+      <c r="B239"/>
+      <c r="C239" t="s">
+        <v>12</v>
+      </c>
+      <c r="D239" t="s">
+        <v>20</v>
+      </c>
+      <c r="E239"/>
+      <c r="F239" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="G239" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="H239" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" ht="13.5" customHeight="1">
       <c r="A240" s="10"/>
       <c r="B240" s="10"/>
       <c r="C240" s="10"/>
@@ -9537,7 +9581,7 @@
       <c r="H240" s="10"/>
       <c r="I240" s="10"/>
     </row>
-    <row r="241" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" ht="13.5" customHeight="1">
       <c r="A241" s="10"/>
       <c r="B241" s="10"/>
       <c r="C241" s="10"/>
@@ -9548,7 +9592,7 @@
       <c r="H241" s="10"/>
       <c r="I241" s="10"/>
     </row>
-    <row r="242" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" ht="13.5" customHeight="1">
       <c r="A242" s="10"/>
       <c r="B242" s="10"/>
       <c r="C242" s="10"/>
@@ -9559,7 +9603,7 @@
       <c r="H242" s="10"/>
       <c r="I242" s="10"/>
     </row>
-    <row r="243" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" ht="13.5" customHeight="1">
       <c r="A243" s="10"/>
       <c r="B243" s="10"/>
       <c r="C243" s="10"/>
@@ -9570,7 +9614,7 @@
       <c r="H243" s="10"/>
       <c r="I243" s="10"/>
     </row>
-    <row r="244" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="13.5" customHeight="1">
       <c r="A244" s="10"/>
       <c r="B244" s="10"/>
       <c r="C244" s="10"/>
@@ -9581,7 +9625,7 @@
       <c r="H244" s="10"/>
       <c r="I244" s="10"/>
     </row>
-    <row r="245" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="13.5" customHeight="1">
       <c r="A245" s="10"/>
       <c r="B245" s="10"/>
       <c r="C245" s="10"/>
@@ -9592,7 +9636,7 @@
       <c r="H245" s="10"/>
       <c r="I245" s="10"/>
     </row>
-    <row r="246" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" ht="13.5" customHeight="1">
       <c r="A246" s="10"/>
       <c r="B246" s="10"/>
       <c r="C246" s="10"/>
@@ -9603,7 +9647,7 @@
       <c r="H246" s="10"/>
       <c r="I246" s="10"/>
     </row>
-    <row r="247" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" ht="13.5" customHeight="1">
       <c r="A247" s="10"/>
       <c r="B247" s="10"/>
       <c r="C247" s="10"/>
@@ -9614,7 +9658,7 @@
       <c r="H247" s="10"/>
       <c r="I247" s="10"/>
     </row>
-    <row r="248" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" ht="13.5" customHeight="1">
       <c r="A248" s="10"/>
       <c r="B248" s="10"/>
       <c r="C248" s="10"/>
@@ -9625,7 +9669,7 @@
       <c r="H248" s="10"/>
       <c r="I248" s="10"/>
     </row>
-    <row r="249" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" ht="13.5" customHeight="1">
       <c r="A249" s="10"/>
       <c r="B249" s="10"/>
       <c r="C249" s="10"/>
@@ -9636,7 +9680,7 @@
       <c r="H249" s="10"/>
       <c r="I249" s="10"/>
     </row>
-    <row r="250" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" ht="13.5" customHeight="1">
       <c r="A250" s="10"/>
       <c r="B250" s="10"/>
       <c r="C250" s="10"/>
@@ -9647,7 +9691,7 @@
       <c r="H250" s="10"/>
       <c r="I250" s="10"/>
     </row>
-    <row r="251" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" ht="13.5" customHeight="1">
       <c r="A251" s="10"/>
       <c r="B251" s="10"/>
       <c r="C251" s="10"/>
@@ -9658,7 +9702,7 @@
       <c r="H251" s="10"/>
       <c r="I251" s="10"/>
     </row>
-    <row r="252" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" ht="13.5" customHeight="1">
       <c r="A252" s="78"/>
       <c r="B252" s="10"/>
       <c r="C252" s="10"/>
@@ -9669,7 +9713,7 @@
       <c r="H252" s="10"/>
       <c r="I252" s="10"/>
     </row>
-    <row r="253" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" ht="13.5" customHeight="1">
       <c r="A253" s="79"/>
       <c r="B253" s="21"/>
       <c r="C253" s="10"/>
@@ -9696,7 +9740,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="8.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" style="1" customWidth="1"/>
@@ -9706,7 +9750,7 @@
     <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -9714,7 +9758,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -9722,7 +9766,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="78"/>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -9730,7 +9774,7 @@
       <c r="E3" s="80"/>
       <c r="F3" s="79"/>
     </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -9738,7 +9782,7 @@
       <c r="E4" s="80"/>
       <c r="F4" s="79"/>
     </row>
-    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -9746,7 +9790,7 @@
       <c r="E5" s="80"/>
       <c r="F5" s="79"/>
     </row>
-    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="78"/>
@@ -9754,7 +9798,7 @@
       <c r="E6" s="80"/>
       <c r="F6" s="79"/>
     </row>
-    <row r="7" spans="1:6" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="137.25" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="80"/>
       <c r="C7" s="12" t="s">
@@ -9764,7 +9808,7 @@
       <c r="E7" s="80"/>
       <c r="F7" s="79"/>
     </row>
-    <row r="8" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30.75" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="80"/>
       <c r="C8" s="79"/>
@@ -9774,7 +9818,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="80"/>
       <c r="C9" s="79"/>
@@ -9782,7 +9826,7 @@
       <c r="E9" s="80"/>
       <c r="F9" s="79"/>
     </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="80"/>
       <c r="C10" s="79"/>
@@ -9790,7 +9834,7 @@
       <c r="E10" s="80"/>
       <c r="F10" s="79"/>
     </row>
-    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="80"/>
       <c r="C11" s="79"/>
@@ -9798,7 +9842,7 @@
       <c r="E11" s="80"/>
       <c r="F11" s="79"/>
     </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="80"/>
       <c r="C12" s="79"/>
@@ -9806,7 +9850,7 @@
       <c r="E12" s="80"/>
       <c r="F12" s="79"/>
     </row>
-    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="80"/>
       <c r="C13" s="79"/>
@@ -9814,7 +9858,7 @@
       <c r="E13" s="80"/>
       <c r="F13" s="79"/>
     </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="80"/>
       <c r="C14" s="79"/>
@@ -9822,7 +9866,7 @@
       <c r="E14" s="80"/>
       <c r="F14" s="79"/>
     </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="80"/>
       <c r="C15" s="79"/>
@@ -9830,7 +9874,7 @@
       <c r="E15" s="80"/>
       <c r="F15" s="79"/>
     </row>
-    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="13.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="80"/>
       <c r="C16" s="79"/>
@@ -9840,7 +9884,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="80"/>
       <c r="C17" s="79"/>

</xml_diff>